<commit_message>
finished BE overlay, fixed Intake metric, some bug fixes
Intake metric was just the milligrams intaken, needed to divide it by the animal weight
</commit_message>
<xml_diff>
--- a/All Figures/Run_all_all_exclusions/Behavior Tables/run_all_exp_BE_GroupStats.xlsx
+++ b/All Figures/Run_all_all_exclusions/Behavior Tables/run_all_exp_BE_GroupStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="392" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1568" uniqueCount="20">
   <si>
     <t>Sex</t>
   </si>
@@ -139,7 +139,7 @@
     <col min="13" max="13" width="13.85546875" customWidth="true"/>
     <col min="14" max="14" width="12.7109375" customWidth="true"/>
     <col min="15" max="15" width="12.7109375" customWidth="true"/>
-    <col min="16" max="16" width="12.7109375" customWidth="true"/>
+    <col min="16" max="16" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -236,10 +236,10 @@
         <v>28.17008898274139</v>
       </c>
       <c r="O2" s="0">
-        <v>17.797383333333332</v>
+        <v>662.60393509215135</v>
       </c>
       <c r="P2" s="0">
-        <v>5.5503888358034086</v>
+        <v>192.7298011765437</v>
       </c>
     </row>
     <row r="3">
@@ -286,10 +286,10 @@
         <v>46.771220369617254</v>
       </c>
       <c r="O3" s="0">
-        <v>25.457016666666664</v>
+        <v>954.82091884984868</v>
       </c>
       <c r="P3" s="0">
-        <v>9.1508001610459733</v>
+        <v>344.05848332991911</v>
       </c>
     </row>
     <row r="4">
@@ -336,10 +336,10 @@
         <v>19.421020773283747</v>
       </c>
       <c r="O4" s="0">
-        <v>21.401916666666668</v>
+        <v>812.07754296646465</v>
       </c>
       <c r="P4" s="0">
-        <v>7.4461323529739296</v>
+        <v>283.08670479648754</v>
       </c>
     </row>
     <row r="5">
@@ -386,10 +386,10 @@
         <v>29.080670626166775</v>
       </c>
       <c r="O5" s="0">
-        <v>24.893808333333336</v>
+        <v>955.27029418837765</v>
       </c>
       <c r="P5" s="0">
-        <v>7.2093066662228491</v>
+        <v>279.45777242579493</v>
       </c>
     </row>
     <row r="6">
@@ -436,10 +436,10 @@
         <v>30.393238392333579</v>
       </c>
       <c r="O6" s="0">
-        <v>23.542108333333335</v>
+        <v>899.30636025498472</v>
       </c>
       <c r="P6" s="0">
-        <v>5.6654696736010948</v>
+        <v>219.30690905617593</v>
       </c>
     </row>
     <row r="7">
@@ -486,10 +486,10 @@
         <v>11.855889757714809</v>
       </c>
       <c r="O7" s="0">
-        <v>27.371924999999994</v>
+        <v>1038.636728649863</v>
       </c>
       <c r="P7" s="0">
-        <v>6.2964942206818204</v>
+        <v>243.52309346660232</v>
       </c>
     </row>
     <row r="8">
@@ -536,10 +536,10 @@
         <v>16.268232736041377</v>
       </c>
       <c r="O8" s="0">
-        <v>27.484566666666669</v>
+        <v>1048.1940092526545</v>
       </c>
       <c r="P8" s="0">
-        <v>5.3329073158356071</v>
+        <v>217.04241147763923</v>
       </c>
     </row>
     <row r="9">
@@ -586,10 +586,10 @@
         <v>10.214010443335667</v>
       </c>
       <c r="O9" s="0">
-        <v>33.116650000000007</v>
+        <v>1286.0533069705627</v>
       </c>
       <c r="P9" s="0">
-        <v>9.4342739556364368</v>
+        <v>369.79571776552183</v>
       </c>
     </row>
     <row r="10">
@@ -636,10 +636,10 @@
         <v>18.319059896156464</v>
       </c>
       <c r="O10" s="0">
-        <v>25.231733333333334</v>
+        <v>943.99066899691809</v>
       </c>
       <c r="P10" s="0">
-        <v>4.8688878463830498</v>
+        <v>181.66081318784734</v>
       </c>
     </row>
     <row r="11">
@@ -686,10 +686,10 @@
         <v>10.646090621035395</v>
       </c>
       <c r="O11" s="0">
-        <v>21.627200000000002</v>
+        <v>810.31570844193584</v>
       </c>
       <c r="P11" s="0">
-        <v>4.4676174480330895</v>
+        <v>169.81642932644624</v>
       </c>
     </row>
     <row r="12">
@@ -736,10 +736,10 @@
         <v>8.2357387455404538</v>
       </c>
       <c r="O12" s="0">
-        <v>22.077766666666673</v>
+        <v>805.07085469088599</v>
       </c>
       <c r="P12" s="0">
-        <v>4.3045680006619991</v>
+        <v>160.90806161211731</v>
       </c>
     </row>
     <row r="13">
@@ -786,10 +786,10 @@
         <v>7.1178363484561382</v>
       </c>
       <c r="O13" s="0">
-        <v>25.794941666666674</v>
+        <v>925.89455499344774</v>
       </c>
       <c r="P13" s="0">
-        <v>5.5469587877865818</v>
+        <v>196.74481614021289</v>
       </c>
     </row>
     <row r="14">
@@ -836,10 +836,10 @@
         <v>46.941755090534691</v>
       </c>
       <c r="O14" s="0">
-        <v>24.217958333333339</v>
+        <v>885.88373992487504</v>
       </c>
       <c r="P14" s="0">
-        <v>5.7165456667659855</v>
+        <v>216.88905013462497</v>
       </c>
     </row>
     <row r="15">
@@ -886,10 +886,10 @@
         <v>18.239459922234531</v>
       </c>
       <c r="O15" s="0">
-        <v>19.824933333333334</v>
+        <v>713.65236589105518</v>
       </c>
       <c r="P15" s="0">
-        <v>4.7216760112006284</v>
+        <v>168.38894238238058</v>
       </c>
     </row>
     <row r="16">
@@ -936,10 +936,10 @@
         <v>8.2433142333508052</v>
       </c>
       <c r="O16" s="0">
-        <v>25.457016666666661</v>
+        <v>924.25520616131644</v>
       </c>
       <c r="P16" s="0">
-        <v>5.3909899847272298</v>
+        <v>202.33334121095055</v>
       </c>
     </row>
     <row r="17">
@@ -986,10 +986,10 @@
         <v>7.4392117706602328</v>
       </c>
       <c r="O17" s="0">
-        <v>102.34782750000002</v>
+        <v>3677.2398080981197</v>
       </c>
       <c r="P17" s="0">
-        <v>40.510185730720508</v>
+        <v>1513.1260728334094</v>
       </c>
     </row>
     <row r="18">
@@ -1036,10 +1036,10 @@
         <v>41.806131708625848</v>
       </c>
       <c r="O18" s="0">
-        <v>50.286458333333336</v>
+        <v>1790.6868914744034</v>
       </c>
       <c r="P18" s="0">
-        <v>16.424235023692233</v>
+        <v>586.95848872727743</v>
       </c>
     </row>
     <row r="19">
@@ -1086,10 +1086,10 @@
         <v>34.255440299995634</v>
       </c>
       <c r="O19" s="0">
-        <v>24.105316666666667</v>
+        <v>855.41816498198102</v>
       </c>
       <c r="P19" s="0">
-        <v>3.505244399204793</v>
+        <v>125.29036696573741</v>
       </c>
     </row>
     <row r="20">
@@ -1136,10 +1136,10 @@
         <v>18.115905248724573</v>
       </c>
       <c r="O20" s="0">
-        <v>16.992799999999995</v>
+        <v>604.2894515648785</v>
       </c>
       <c r="P20" s="0">
-        <v>3.1661834204798072</v>
+        <v>114.28087933685454</v>
       </c>
     </row>
     <row r="21">
@@ -1186,10 +1186,10 @@
         <v>11.68443843648136</v>
       </c>
       <c r="O21" s="0">
-        <v>16.249365000000001</v>
+        <v>553.92428301774737</v>
       </c>
       <c r="P21" s="0">
-        <v>4.7614553727991975</v>
+        <v>168.88364808995513</v>
       </c>
     </row>
     <row r="22">
@@ -1236,10 +1236,10 @@
         <v>26.447986623194296</v>
       </c>
       <c r="O22" s="0">
-        <v>19.599650000000004</v>
+        <v>691.43918742017877</v>
       </c>
       <c r="P22" s="0">
-        <v>5.2537751476914201</v>
+        <v>183.26835110673994</v>
       </c>
     </row>
     <row r="23">
@@ -1286,10 +1286,10 @@
         <v>19.321804014096223</v>
       </c>
       <c r="O23" s="0">
-        <v>15.206624999999999</v>
+        <v>538.38801644316732</v>
       </c>
       <c r="P23" s="0">
-        <v>3.4532656679040783</v>
+        <v>122.7575456246515</v>
       </c>
     </row>
     <row r="24">
@@ -1336,10 +1336,10 @@
         <v>5.2854190521024105</v>
       </c>
       <c r="O24" s="0">
-        <v>4.5619875000000008</v>
+        <v>135.8047085719584</v>
       </c>
       <c r="P24" s="0">
-        <v>1.5733873434905499</v>
+        <v>47.440191316611013</v>
       </c>
     </row>
     <row r="25">
@@ -1386,10 +1386,10 @@
         <v>4.462195137769176</v>
       </c>
       <c r="O25" s="0">
-        <v>2.0275500000000002</v>
+        <v>84.740911693379076</v>
       </c>
       <c r="P25" s="0">
-        <v>0.82355268644360857</v>
+        <v>31.606962889645008</v>
       </c>
     </row>
     <row r="26">
@@ -1436,10 +1436,10 @@
         <v>2.4347657100624729</v>
       </c>
       <c r="O26" s="0">
-        <v>6.9837833333333341</v>
+        <v>389.01613188944566</v>
       </c>
       <c r="P26" s="0">
-        <v>3.2126670042390426</v>
+        <v>183.35353000496002</v>
       </c>
     </row>
     <row r="27">
@@ -1486,10 +1486,10 @@
         <v>5.4995890185780514</v>
       </c>
       <c r="O27" s="0">
-        <v>12.728508333333332</v>
+        <v>705.63269952560256</v>
       </c>
       <c r="P27" s="0">
-        <v>4.9955254394437896</v>
+        <v>283.36501249227683</v>
       </c>
     </row>
     <row r="28">
@@ -1536,10 +1536,10 @@
         <v>1.5925464164131875</v>
       </c>
       <c r="O28" s="0">
-        <v>15.769833333333333</v>
+        <v>877.9498416654792</v>
       </c>
       <c r="P28" s="0">
-        <v>5.0420659305717459</v>
+        <v>285.69945366645271</v>
       </c>
     </row>
     <row r="29">
@@ -1586,10 +1586,10 @@
         <v>2.8831593554079551</v>
       </c>
       <c r="O29" s="0">
-        <v>23.204183333333333</v>
+        <v>1288.3494900344381</v>
       </c>
       <c r="P29" s="0">
-        <v>6.2273256862923567</v>
+        <v>353.26382814377189</v>
       </c>
     </row>
     <row r="30">
@@ -1636,10 +1636,10 @@
         <v>0.83168206977904935</v>
       </c>
       <c r="O30" s="0">
-        <v>22.866258333333334</v>
+        <v>1261.6898732778029</v>
       </c>
       <c r="P30" s="0">
-        <v>6.6997908066217775</v>
+        <v>374.08152310602077</v>
       </c>
     </row>
     <row r="31">
@@ -1686,10 +1686,10 @@
         <v>1.3793186977299656</v>
       </c>
       <c r="O31" s="0">
-        <v>23.992675000000002</v>
+        <v>1320.6882719499338</v>
       </c>
       <c r="P31" s="0">
-        <v>6.4141042752520656</v>
+        <v>357.81913928136248</v>
       </c>
     </row>
     <row r="32">
@@ -1736,10 +1736,10 @@
         <v>0.77348230650469929</v>
       </c>
       <c r="O32" s="0">
-        <v>29.399475000000006</v>
+        <v>1619.2040325628702</v>
       </c>
       <c r="P32" s="0">
-        <v>7.7793953221345715</v>
+        <v>439.71763724873756</v>
       </c>
     </row>
     <row r="33">
@@ -1786,10 +1786,10 @@
         <v>1.9363214968675284</v>
       </c>
       <c r="O33" s="0">
-        <v>32.66608333333334</v>
+        <v>1792.1935255685628</v>
       </c>
       <c r="P33" s="0">
-        <v>6.7888111450501087</v>
+        <v>382.97866840220581</v>
       </c>
     </row>
     <row r="34">
@@ -1836,10 +1836,10 @@
         <v>0.59909651846691225</v>
       </c>
       <c r="O34" s="0">
-        <v>34.806275000000007</v>
+        <v>1906.024291026303</v>
       </c>
       <c r="P34" s="0">
-        <v>6.7526093457553564</v>
+        <v>379.00519413871899</v>
       </c>
     </row>
     <row r="35">
@@ -1886,10 +1886,10 @@
         <v>0.56254067183450229</v>
       </c>
       <c r="O35" s="0">
-        <v>28.723625000000002</v>
+        <v>1572.2573155346765</v>
       </c>
       <c r="P35" s="0">
-        <v>7.5224978259876325</v>
+        <v>424.86006599213249</v>
       </c>
     </row>
     <row r="36">
@@ -1936,10 +1936,10 @@
         <v>0.50135291339695542</v>
       </c>
       <c r="O36" s="0">
-        <v>28.047775000000001</v>
+        <v>1528.4838728682173</v>
       </c>
       <c r="P36" s="0">
-        <v>5.5110760195309636</v>
+        <v>309.94354488991985</v>
       </c>
     </row>
     <row r="37">
@@ -1986,10 +1986,10 @@
         <v>0.90052187169582865</v>
       </c>
       <c r="O37" s="0">
-        <v>34.580991666666669</v>
+        <v>1890.5007396328685</v>
       </c>
       <c r="P37" s="0">
-        <v>8.7512564910093396</v>
+        <v>493.27112163403336</v>
       </c>
     </row>
     <row r="38">
@@ -2036,10 +2036,10 @@
         <v>1.2243806140286655</v>
       </c>
       <c r="O38" s="0">
-        <v>36.157975</v>
+        <v>1989.2625158770416</v>
       </c>
       <c r="P38" s="0">
-        <v>12.329316777748863</v>
+        <v>701.9557933432659</v>
       </c>
     </row>
     <row r="39">
@@ -2086,10 +2086,10 @@
         <v>1.2983085032609183</v>
       </c>
       <c r="O39" s="0">
-        <v>33.905141666666665</v>
+        <v>1855.3261441497395</v>
       </c>
       <c r="P39" s="0">
-        <v>8.2949083042629272</v>
+        <v>467.0670608117893</v>
       </c>
     </row>
     <row r="40">
@@ -2136,10 +2136,10 @@
         <v>1.9379461798804087</v>
       </c>
       <c r="O40" s="0">
-        <v>74.304880000000011</v>
+        <v>3940.6454600786842</v>
       </c>
       <c r="P40" s="0">
-        <v>22.088775518107095</v>
+        <v>1143.1339665169069</v>
       </c>
     </row>
     <row r="41">
@@ -2186,10 +2186,10 @@
         <v>0.7730841890471889</v>
       </c>
       <c r="O41" s="0">
-        <v>38.016562500000006</v>
+        <v>2036.2425266360976</v>
       </c>
       <c r="P41" s="0">
-        <v>6.5237925874144125</v>
+        <v>354.77592678409894</v>
       </c>
     </row>
     <row r="42">
@@ -2236,10 +2236,10 @@
         <v>1.0402034050474773</v>
       </c>
       <c r="O42" s="0">
-        <v>32.215516666666673</v>
+        <v>1727.8118176156586</v>
       </c>
       <c r="P42" s="0">
-        <v>5.3419838757632121</v>
+        <v>291.8278835381451</v>
       </c>
     </row>
     <row r="43">
@@ -2286,10 +2286,10 @@
         <v>1.1639431001467764</v>
       </c>
       <c r="O43" s="0">
-        <v>27.548933333333334</v>
+        <v>1474.5796351149672</v>
       </c>
       <c r="P43" s="0">
-        <v>4.122756830034481</v>
+        <v>225.57646625049392</v>
       </c>
     </row>
     <row r="44">
@@ -2336,10 +2336,10 @@
         <v>6.7686942936056207</v>
       </c>
       <c r="O44" s="0">
-        <v>23.435903333333339</v>
+        <v>1250.9863792015792</v>
       </c>
       <c r="P44" s="0">
-        <v>4.4027129360366493</v>
+        <v>234.1696268731057</v>
       </c>
     </row>
     <row r="45">
@@ -2386,10 +2386,10 @@
         <v>0.40829587589885746</v>
       </c>
       <c r="O45" s="0">
-        <v>31.258062500000001</v>
+        <v>1661.3108664386739</v>
       </c>
       <c r="P45" s="0">
-        <v>6.4494117230881027</v>
+        <v>349.24687261918882</v>
       </c>
     </row>
     <row r="46">
@@ -2436,10 +2436,10 @@
         <v>0.30768442174883209</v>
       </c>
       <c r="O46" s="0">
-        <v>23.147862500000002</v>
+        <v>1239.3874065421342</v>
       </c>
       <c r="P46" s="0">
-        <v>6.9603527145832373</v>
+        <v>377.93930868525126</v>
       </c>
     </row>
     <row r="47">
@@ -2486,10 +2486,10 @@
         <v>20.383229336232841</v>
       </c>
       <c r="O47" s="0">
-        <v>20.275500000000001</v>
+        <v>553.6875854764379</v>
       </c>
       <c r="P47" s="0">
-        <v>6.2076605934632392</v>
+        <v>167.15378413723346</v>
       </c>
     </row>
     <row r="48">
@@ -2536,10 +2536,10 @@
         <v>25.453241569681712</v>
       </c>
       <c r="O48" s="0">
-        <v>13.404358333333334</v>
+        <v>381.1568442259404</v>
       </c>
       <c r="P48" s="0">
-        <v>3.4157467888034327</v>
+        <v>104.64998514589992</v>
       </c>
     </row>
     <row r="49">
@@ -2586,10 +2586,10 @@
         <v>14.589387828309476</v>
       </c>
       <c r="O49" s="0">
-        <v>12.615866666666667</v>
+        <v>345.04235611416243</v>
       </c>
       <c r="P49" s="0">
-        <v>3.5229693176898151</v>
+        <v>96.40136943660292</v>
       </c>
     </row>
     <row r="50">
@@ -2636,10 +2636,10 @@
         <v>27.586682182361844</v>
       </c>
       <c r="O50" s="0">
-        <v>14.418133333333335</v>
+        <v>405.18633241906849</v>
       </c>
       <c r="P50" s="0">
-        <v>3.4595348247541708</v>
+        <v>100.57567248092614</v>
       </c>
     </row>
     <row r="51">
@@ -2686,10 +2686,10 @@
         <v>24.072270140658045</v>
       </c>
       <c r="O51" s="0">
-        <v>18.135308333333331</v>
+        <v>502.86135057239034</v>
       </c>
       <c r="P51" s="0">
-        <v>5.3019960519808915</v>
+        <v>143.23164367131866</v>
       </c>
     </row>
     <row r="52">
@@ -2736,10 +2736,10 @@
         <v>6.2548712292345199</v>
       </c>
       <c r="O52" s="0">
-        <v>23.542108333333335</v>
+        <v>609.86578383430708</v>
       </c>
       <c r="P52" s="0">
-        <v>5.7431184770895713</v>
+        <v>140.91601621588853</v>
       </c>
     </row>
     <row r="53">
@@ -2786,10 +2786,10 @@
         <v>8.5662356551486187</v>
       </c>
       <c r="O53" s="0">
-        <v>23.767391666666668</v>
+        <v>628.74599378661958</v>
       </c>
       <c r="P53" s="0">
-        <v>6.4899055687958702</v>
+        <v>178.18833917324125</v>
       </c>
     </row>
     <row r="54">
@@ -2836,10 +2836,10 @@
         <v>11.966468207089113</v>
       </c>
       <c r="O54" s="0">
-        <v>28.216737500000001</v>
+        <v>777.90386346391608</v>
       </c>
       <c r="P54" s="0">
-        <v>9.0510475520188418</v>
+        <v>254.56241851651271</v>
       </c>
     </row>
     <row r="55">
@@ -2886,10 +2886,10 @@
         <v>66.15666070775147</v>
       </c>
       <c r="O55" s="0">
-        <v>30.863816666666668</v>
+        <v>819.87427860569107</v>
       </c>
       <c r="P55" s="0">
-        <v>8.1201495997735194</v>
+        <v>227.33965868704396</v>
       </c>
     </row>
     <row r="56">
@@ -2936,10 +2936,10 @@
         <v>17.201600851484219</v>
       </c>
       <c r="O56" s="0">
-        <v>30.638533333333339</v>
+        <v>800.55066289636613</v>
       </c>
       <c r="P56" s="0">
-        <v>9.1696883211739966</v>
+        <v>249.9419719018741</v>
       </c>
     </row>
     <row r="57">
@@ -2986,10 +2986,10 @@
         <v>34.266463994248042</v>
       </c>
       <c r="O57" s="0">
-        <v>27.034000000000002</v>
+        <v>692.46714717198768</v>
       </c>
       <c r="P57" s="0">
-        <v>6.3356670626531413</v>
+        <v>161.54193206805655</v>
       </c>
     </row>
     <row r="58">
@@ -3036,10 +3036,10 @@
         <v>36.283643103522174</v>
       </c>
       <c r="O58" s="0">
-        <v>29.624758333333336</v>
+        <v>751.01425229442748</v>
       </c>
       <c r="P58" s="0">
-        <v>7.0442195047521103</v>
+        <v>169.98534173436673</v>
       </c>
     </row>
     <row r="59">
@@ -3086,10 +3086,10 @@
         <v>142.69083084872554</v>
       </c>
       <c r="O59" s="0">
-        <v>30.187966666666668</v>
+        <v>768.38054864868434</v>
       </c>
       <c r="P59" s="0">
-        <v>6.3188953991823675</v>
+        <v>156.08475178294529</v>
       </c>
     </row>
     <row r="60">
@@ -3136,10 +3136,10 @@
         <v>37.899407884773794</v>
       </c>
       <c r="O60" s="0">
-        <v>28.047775000000001</v>
+        <v>716.54902569990747</v>
       </c>
       <c r="P60" s="0">
-        <v>6.4742462086930646</v>
+        <v>160.87595102179287</v>
       </c>
     </row>
     <row r="61">
@@ -3186,10 +3186,10 @@
         <v>9.133318217493688</v>
       </c>
       <c r="O61" s="0">
-        <v>25.344374999999999</v>
+        <v>648.17679295783716</v>
       </c>
       <c r="P61" s="0">
-        <v>6.2634328516388393</v>
+        <v>159.02501919219446</v>
       </c>
     </row>
     <row r="62">
@@ -3236,10 +3236,10 @@
         <v>14.421584017528945</v>
       </c>
       <c r="O62" s="0">
-        <v>65.374005000000011</v>
+        <v>1759.5391597467874</v>
       </c>
       <c r="P62" s="0">
-        <v>14.888601685713303</v>
+        <v>427.54812947467633</v>
       </c>
     </row>
     <row r="63">
@@ -3286,10 +3286,10 @@
         <v>31.845509543742029</v>
       </c>
       <c r="O63" s="0">
-        <v>37.21197916666668</v>
+        <v>964.25151149946817</v>
       </c>
       <c r="P63" s="0">
-        <v>7.3708852004182415</v>
+        <v>200.6676595603054</v>
       </c>
     </row>
     <row r="64">
@@ -3336,10 +3336,10 @@
         <v>8.3592339117619492</v>
       </c>
       <c r="O64" s="0">
-        <v>26.583433333333335</v>
+        <v>675.02612769402242</v>
       </c>
       <c r="P64" s="0">
-        <v>6.886987237177844</v>
+        <v>168.70970064698326</v>
       </c>
     </row>
     <row r="65">
@@ -3386,10 +3386,10 @@
         <v>33.956023100731898</v>
       </c>
       <c r="O65" s="0">
-        <v>20.082400000000003</v>
+        <v>521.81100256789966</v>
       </c>
       <c r="P65" s="0">
-        <v>5.6102818601477615</v>
+        <v>150.53361893188935</v>
       </c>
     </row>
     <row r="66">
@@ -3436,10 +3436,10 @@
         <v>7.3245710067255274</v>
       </c>
       <c r="O66" s="0">
-        <v>14.904101666666667</v>
+        <v>435.84169482412852</v>
       </c>
       <c r="P66" s="0">
-        <v>4.4248993625470678</v>
+        <v>157.17834068467118</v>
       </c>
     </row>
     <row r="67">
@@ -3486,10 +3486,10 @@
         <v>74.143200287076453</v>
       </c>
       <c r="O67" s="0">
-        <v>27.878812500000002</v>
+        <v>689.819406004916</v>
       </c>
       <c r="P67" s="0">
-        <v>10.710333973908387</v>
+        <v>255.33802191077586</v>
       </c>
     </row>
     <row r="68">
@@ -3536,10 +3536,10 @@
         <v>3.6997937293116876</v>
       </c>
       <c r="O68" s="0">
-        <v>25.513337500000002</v>
+        <v>635.98771358848114</v>
       </c>
       <c r="P68" s="0">
-        <v>9.2012010696379321</v>
+        <v>222.63633082904892</v>
       </c>
     </row>
     <row r="69">
@@ -3586,10 +3586,10 @@
         <v>5.283104444708286</v>
       </c>
       <c r="O69" s="0">
-        <v>2.0275499999999997</v>
+        <v>101.24748633857224</v>
       </c>
       <c r="P69" s="0">
-        <v>1.198153990520417</v>
+        <v>57.870559127304546</v>
       </c>
     </row>
     <row r="70">
@@ -3636,10 +3636,10 @@
         <v>6.5579711378172822</v>
       </c>
       <c r="O70" s="0">
-        <v>1.0137750000000001</v>
+        <v>43.446153732682433</v>
       </c>
       <c r="P70" s="0">
-        <v>0.47426385910086216</v>
+        <v>19.481130681009965</v>
       </c>
     </row>
     <row r="71">
@@ -3686,10 +3686,10 @@
         <v>3.4509399525636488</v>
       </c>
       <c r="O71" s="0">
-        <v>5.2941583333333337</v>
+        <v>233.09003714234134</v>
       </c>
       <c r="P71" s="0">
-        <v>1.6676362630008694</v>
+        <v>73.835653805418957</v>
       </c>
     </row>
     <row r="72">
@@ -3736,10 +3736,10 @@
         <v>4.1859655844640864</v>
       </c>
       <c r="O72" s="0">
-        <v>11.940016666666665</v>
+        <v>525.08735140180067</v>
       </c>
       <c r="P72" s="0">
-        <v>3.3806150778177471</v>
+        <v>147.59747939020144</v>
       </c>
     </row>
     <row r="73">
@@ -3786,10 +3786,10 @@
         <v>21.146924423285945</v>
       </c>
       <c r="O73" s="0">
-        <v>16.558325</v>
+        <v>729.78353756724982</v>
       </c>
       <c r="P73" s="0">
-        <v>4.3835623611175905</v>
+        <v>188.88548914135833</v>
       </c>
     </row>
     <row r="74">
@@ -3836,10 +3836,10 @@
         <v>1.458890054541055</v>
       </c>
       <c r="O74" s="0">
-        <v>28.610983333333337</v>
+        <v>1269.5068328253928</v>
       </c>
       <c r="P74" s="0">
-        <v>5.7271291649697824</v>
+        <v>250.69678692666332</v>
       </c>
     </row>
     <row r="75">
@@ -3886,10 +3886,10 @@
         <v>1.5629559611701105</v>
       </c>
       <c r="O75" s="0">
-        <v>32.891366666666663</v>
+        <v>1442.867264171098</v>
       </c>
       <c r="P75" s="0">
-        <v>5.5963341485586113</v>
+        <v>248.35870839625946</v>
       </c>
     </row>
     <row r="76">
@@ -3936,10 +3936,10 @@
         <v>1.377233915733419</v>
       </c>
       <c r="O76" s="0">
-        <v>31.990233333333336</v>
+        <v>1396.8787713297468</v>
       </c>
       <c r="P76" s="0">
-        <v>4.4031222633616611</v>
+        <v>197.78485031247564</v>
       </c>
     </row>
     <row r="77">
@@ -3986,10 +3986,10 @@
         <v>0.64719308633567585</v>
       </c>
       <c r="O77" s="0">
-        <v>34.918916666666668</v>
+        <v>1518.7456781473618</v>
       </c>
       <c r="P77" s="0">
-        <v>3.9647772034892554</v>
+        <v>173.44180797259369</v>
       </c>
     </row>
     <row r="78">
@@ -4036,10 +4036,10 @@
         <v>0.50240103972519146</v>
       </c>
       <c r="O78" s="0">
-        <v>34.13042500000001</v>
+        <v>1493.6812088852755</v>
       </c>
       <c r="P78" s="0">
-        <v>4.2260076809099454</v>
+        <v>191.56076941151991</v>
       </c>
     </row>
     <row r="79">
@@ -4086,10 +4086,10 @@
         <v>0.20850185525397355</v>
       </c>
       <c r="O79" s="0">
-        <v>32.328158333333334</v>
+        <v>1416.2329313795578</v>
       </c>
       <c r="P79" s="0">
-        <v>3.8823141133564167</v>
+        <v>177.05695535930957</v>
       </c>
     </row>
     <row r="80">
@@ -4136,10 +4136,10 @@
         <v>0.31164511080970914</v>
       </c>
       <c r="O80" s="0">
-        <v>36.383258333333337</v>
+        <v>1588.540998948022</v>
       </c>
       <c r="P80" s="0">
-        <v>4.39407514643226</v>
+        <v>200.41675457017672</v>
       </c>
     </row>
     <row r="81">
@@ -4186,10 +4186,10 @@
         <v>0.36973042072266604</v>
       </c>
       <c r="O81" s="0">
-        <v>36.383258333333337</v>
+        <v>1591.2319348276831</v>
       </c>
       <c r="P81" s="0">
-        <v>2.6954949923636153</v>
+        <v>127.43491260971827</v>
       </c>
     </row>
     <row r="82">
@@ -4236,10 +4236,10 @@
         <v>0.77012512901209973</v>
       </c>
       <c r="O82" s="0">
-        <v>36.721183333333336</v>
+        <v>1602.2802056376374</v>
       </c>
       <c r="P82" s="0">
-        <v>3.1385688529683775</v>
+        <v>142.86324795189168</v>
       </c>
     </row>
     <row r="83">
@@ -4286,10 +4286,10 @@
         <v>0.29022630161841223</v>
       </c>
       <c r="O83" s="0">
-        <v>40.888925</v>
+        <v>1789.6235796883129</v>
       </c>
       <c r="P83" s="0">
-        <v>3.6419397947390335</v>
+        <v>169.27996207719642</v>
       </c>
     </row>
     <row r="84">
@@ -4336,10 +4336,10 @@
         <v>0.28122686915381523</v>
       </c>
       <c r="O84" s="0">
-        <v>39.537224999999999</v>
+        <v>1728.0761897073371</v>
       </c>
       <c r="P84" s="0">
-        <v>3.458701181804948</v>
+        <v>161.71274297630765</v>
       </c>
     </row>
     <row r="85">
@@ -4386,10 +4386,10 @@
         <v>1.3159350933604834</v>
       </c>
       <c r="O85" s="0">
-        <v>65.016770000000008</v>
+        <v>2803.1554334332782</v>
       </c>
       <c r="P85" s="0">
-        <v>10.364853140140569</v>
+        <v>463.03615246140919</v>
       </c>
     </row>
     <row r="86">
@@ -4436,10 +4436,10 @@
         <v>1.4433190557500086</v>
       </c>
       <c r="O86" s="0">
-        <v>50.286458333333343</v>
+        <v>2163.5786978892343</v>
       </c>
       <c r="P86" s="0">
-        <v>4.7615243891389341</v>
+        <v>213.76418640364801</v>
       </c>
     </row>
     <row r="87">
@@ -4486,10 +4486,10 @@
         <v>0.55115988596114063</v>
       </c>
       <c r="O87" s="0">
-        <v>37.8476</v>
+        <v>1642.3069691780795</v>
       </c>
       <c r="P87" s="0">
-        <v>3.3234931949408568</v>
+        <v>157.68446954082407</v>
       </c>
     </row>
     <row r="88">
@@ -4536,10 +4536,10 @@
         <v>0.22894413031447025</v>
       </c>
       <c r="O88" s="0">
-        <v>29.479933333333335</v>
+        <v>1270.8576160651719</v>
       </c>
       <c r="P88" s="0">
-        <v>2.2615935737725499</v>
+        <v>101.73214796763017</v>
       </c>
     </row>
     <row r="89">
@@ -4586,10 +4586,10 @@
         <v>1.5739655922395606</v>
       </c>
       <c r="O89" s="0">
-        <v>26.72825833333334</v>
+        <v>1150.4877790263338</v>
       </c>
       <c r="P89" s="0">
-        <v>3.3995488231630744</v>
+        <v>141.84579524582941</v>
       </c>
     </row>
     <row r="90">
@@ -4636,10 +4636,10 @@
         <v>0.25920454883653488</v>
       </c>
       <c r="O90" s="0">
-        <v>43.254400000000004</v>
+        <v>1911.6565596553658</v>
       </c>
       <c r="P90" s="0">
-        <v>5.6198403598322964</v>
+        <v>265.98246709956334</v>
       </c>
     </row>
     <row r="91">
@@ -4686,10 +4686,10 @@
         <v>0.35381113144433413</v>
       </c>
       <c r="O91" s="0">
-        <v>29.737400000000004</v>
+        <v>1308.7104571620723</v>
       </c>
       <c r="P91" s="0">
-        <v>4.2206818972175579</v>
+        <v>186.40924439033535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>